<commit_message>
validate excel document upload, handle recieved document upload from department
</commit_message>
<xml_diff>
--- a/resources/data-import-sample.xlsx
+++ b/resources/data-import-sample.xlsx
@@ -5,14 +5,29 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="projects" sheetId="1" r:id="rId4"/>
-    <sheet name="milestones" sheetId="2" r:id="rId5"/>
+    <sheet name="Projects" sheetId="1" r:id="rId4"/>
+    <sheet name="Milestones" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Group 4</t>
+  </si>
+  <si>
+    <t>Group 5</t>
+  </si>
   <si>
     <t>UID</t>
   </si>
@@ -95,6 +110,18 @@
     <t>Change in latest start date</t>
   </si>
   <si>
+    <t>Some description about Project UID</t>
+  </si>
+  <si>
+    <t>Column description</t>
+  </si>
+  <si>
+    <t>[Set by CO]</t>
+  </si>
+  <si>
+    <t>Column field type</t>
+  </si>
+  <si>
     <t>PRO-01</t>
   </si>
   <si>
@@ -258,6 +285,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>The UID of the project these milestones cover</t>
   </si>
   <si>
     <t>MIL-01-01</t>
@@ -358,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -379,6 +409,19 @@
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -416,6 +459,17 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -435,6 +489,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -474,7 +541,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -482,6 +549,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -509,6 +579,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1598,631 +1677,1028 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.3516" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6719" style="1" customWidth="1"/>
-    <col min="13" max="27" width="16.3516" style="1" customWidth="1"/>
-    <col min="28" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="4" width="1.5" style="1" customWidth="1"/>
+    <col min="5" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6719" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="30.3516" style="1" customWidth="1"/>
+    <col min="14" max="14" width="29.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.3516" style="1" customWidth="1"/>
+    <col min="16" max="16" width="30.6719" style="1" customWidth="1"/>
+    <col min="17" max="31" width="16.3516" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="9" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+    </row>
+    <row r="2" ht="9" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+    </row>
+    <row r="3" ht="9" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+    </row>
+    <row r="4" ht="9" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+    </row>
+    <row r="5" ht="36" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+    </row>
+    <row r="6" ht="36" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="F6" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="G6" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="H6" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="I6" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="J6" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="K6" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="N6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="O6" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="P6" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="Q6" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="R6" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="2">
+      <c r="S6" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="2">
+      <c r="T6" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="2">
+      <c r="U6" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="2">
+      <c r="V6" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="2">
+      <c r="W6" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="Y1" t="s" s="2">
+      <c r="X6" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="2">
+      <c r="Y6" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="AA1" t="s" s="2">
+      <c r="Z6" t="s" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="AA6" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="AB6" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="AC6" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="AD6" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="AE6" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="F2" t="s" s="2">
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s" s="2">
+      <c r="F7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="P7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="R7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="T7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="U7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="V7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="W7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="X7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="Y7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="Z7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AA7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AB7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AC7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AD7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AE7" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="I2" t="s" s="2">
+      <c r="F8" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="J2" t="s" s="2">
+      <c r="G8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="P8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="R8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="S8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="T8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="U8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="V8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="W8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="X8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Y8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Z8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AA8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE8" t="s" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="K2" t="s" s="2">
+      <c r="F9" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="L2" t="s" s="2">
+      <c r="G9" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="M2" t="s" s="2">
+      <c r="H9" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="N2" t="s" s="2">
+      <c r="I9" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="O2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Q2" t="s" s="2">
+      <c r="J9" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="R2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA2" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="2">
+      <c r="K9" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="N9" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="O9" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s" s="2">
+      <c r="P9" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="J3" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s" s="2">
+      <c r="Q9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="R9" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="S9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="T9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="U9" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="V9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="W9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="X9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="Y9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="Z9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AA9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AB9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AC9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AD9" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AE9" t="s" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="G10" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="I10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="M10" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R10" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="S10" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="T10" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="U10" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="V10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W10" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="X10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y10" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="Z10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA10" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AC10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE10" t="s" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="J11" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="N11" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="O11" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="P11" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="Q11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="R11" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="S11" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="M3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="O3" t="s" s="2">
+      <c r="T11" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="W11" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="X11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="Y11" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="Z11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AA11" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AB11" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AC11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AD11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AE11" t="s" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="R12" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="P3" t="s" s="2">
+      <c r="S12" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="T12" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="W12" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G13" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="J13" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K13" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="M13" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="N13" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="R13" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="Q3" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="S3" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="T3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="U3" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="V3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="W3" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="X3" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="Y3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="Z3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="AA3" t="s" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J4" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="N4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S4" t="s" s="2">
+      <c r="S13" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="T13" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="W13" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="T4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U4" t="s" s="2">
+      <c r="X13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Y13" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="V4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X4" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="Y4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA4" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="J5" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="P5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="S5" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="T5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="U5" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="V5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="W5" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="X5" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="Y5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="Z5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AA5" t="s" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="O6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="S6" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="T6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="U6" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="V6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="W6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X6" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="Y6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="Z6" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="5"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="8"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="8"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="11"/>
+      <c r="Z13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AA13" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AB13" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AC13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AD13" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE13" t="s" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="7"/>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="11"/>
+    </row>
+    <row r="16" ht="14.7" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="11"/>
+    </row>
+    <row r="17" ht="14.7" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="X5:AE5"/>
+  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2233,249 +2709,371 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="12" customWidth="1"/>
-    <col min="2" max="2" width="23.1719" style="12" customWidth="1"/>
-    <col min="3" max="8" width="16.3516" style="12" customWidth="1"/>
-    <col min="9" max="9" width="30.3516" style="12" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="12" customWidth="1"/>
-    <col min="11" max="256" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="2" width="1.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="16" customWidth="1"/>
+    <col min="4" max="4" width="23.1719" style="16" customWidth="1"/>
+    <col min="5" max="10" width="16.3516" style="16" customWidth="1"/>
+    <col min="11" max="11" width="30.3516" style="16" customWidth="1"/>
+    <col min="12" max="12" width="29.5" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="9" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" ht="9" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" ht="9" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" ht="36" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" ht="36" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="J5" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="L5" t="s" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s" s="2">
+      <c r="J10" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="F1" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G1" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H1" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="I1" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="J1" t="s" s="2">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G2" s="13">
+      <c r="D11" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="I11" s="17">
         <v>0</v>
       </c>
-      <c r="H2" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="G3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="I5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s" s="2">
+      <c r="J11" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="E6" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:L4"/>
+  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>